<commit_message>
modif struct-info about DB
</commit_message>
<xml_diff>
--- a/MetaFiles/DB_Films.xlsx
+++ b/MetaFiles/DB_Films.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\___Code___\__Programing__\AppMyFilms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Study\AppMyFilms\MetaFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8B07BD-CE18-4680-8B69-6B7EA1ACF8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8137C3E7-A9C8-4605-978B-209B383078CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FE7F364-4D14-4A6C-8063-AF17EB6AC720}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{4FE7F364-4D14-4A6C-8063-AF17EB6AC720}"/>
   </bookViews>
   <sheets>
     <sheet name="Films" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Genres" sheetId="3" r:id="rId4"/>
     <sheet name="GenreList" sheetId="4" r:id="rId5"/>
     <sheet name="Description" sheetId="2" r:id="rId6"/>
+    <sheet name="Users" sheetId="8" r:id="rId7"/>
+    <sheet name="ListFilms" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Country</t>
   </si>
@@ -90,6 +92,15 @@
   </si>
   <si>
     <t>DirectorsId</t>
+  </si>
+  <si>
+    <t>IdFilms</t>
+  </si>
+  <si>
+    <t>IdUser</t>
+  </si>
+  <si>
+    <t>UserName</t>
   </si>
 </sst>
 </file>
@@ -484,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4925E81E-0975-489E-BD0A-2880252BCFF3}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -784,4 +795,56 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6025E6D4-82FD-411E-A3FE-92538096F751}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="28.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A117DEE6-3D24-44C5-B098-6B6FBFF94ABC}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="28.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
start add listfilm repo in project
</commit_message>
<xml_diff>
--- a/MetaFiles/DB_Films.xlsx
+++ b/MetaFiles/DB_Films.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Study\AppMyFilms\MetaFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\___Code___\__Programing__\AppMyFilms\MetaFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8137C3E7-A9C8-4605-978B-209B383078CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E441C3F-A9A9-40BC-95E3-E4D1A96824BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{4FE7F364-4D14-4A6C-8063-AF17EB6AC720}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{4FE7F364-4D14-4A6C-8063-AF17EB6AC720}"/>
   </bookViews>
   <sheets>
     <sheet name="Films" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Country</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>UserName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -496,7 +505,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -697,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9B498F-D993-4FA3-9BE0-4B6EFD93C451}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -799,10 +808,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6025E6D4-82FD-411E-A3FE-92538096F751}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -810,12 +819,21 @@
     <col min="1" max="16384" width="28.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -828,7 +846,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>